<commit_message>
ollama, openRouter und shared_logic with gemini-2_5-flash-lite
</commit_message>
<xml_diff>
--- a/data/NET Tubo v2.xlsx
+++ b/data/NET Tubo v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pia\Documents\PhD\Paper\LLM Tumorboard\llmTubo\llmRecom\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pia\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21989B3-BD7E-4846-AA08-BC0CD1D4B6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4EB5E-D8DC-4B83-A7A6-106BB2232AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{8671C793-EBC6-4E35-BB39-8A527F2DCF4A}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="16874" windowHeight="10432" xr2:uid="{8671C793-EBC6-4E35-BB39-8A527F2DCF4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Fragestellung</t>
   </si>
@@ -87,24 +87,6 @@
     <t>PRRT starten.</t>
   </si>
   <si>
-    <t>Handlungsoptionen:</t>
-  </si>
-  <si>
-    <t>Therapie intensivieren</t>
-  </si>
-  <si>
-    <t>Therapie fortführen ohne Intensivierung</t>
-  </si>
-  <si>
-    <t>Therapie deeskalieren</t>
-  </si>
-  <si>
-    <t>konsolidierend Strahlentherapie</t>
-  </si>
-  <si>
-    <t>follow up imaging</t>
-  </si>
-  <si>
     <t>main_diagnosis_text</t>
   </si>
   <si>
@@ -153,7 +135,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,18 +151,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1F497D"/>
-      <name val="Aptos"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -190,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -198,91 +168,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -314,17 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -659,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FE7E66-A423-4825-A285-7BBECB18F444}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -676,164 +555,123 @@
     <col min="7" max="16384" width="10.6640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="1:16" customFormat="1" ht="16.149999999999999" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="N2" s="11" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
+      <c r="E1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="I3" s="14"/>
-      <c r="N3" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="16"/>
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8">
+        <v>12.202400000000001</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="N4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="16"/>
+    <row r="3" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="9">
+        <v>8.2014999999999993</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="N5" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="P5" s="16"/>
+    <row r="4" spans="1:6" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="9">
+        <v>8.2014999999999993</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="N6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="P6" s="16"/>
+    <row r="5" spans="1:6" ht="171" x14ac:dyDescent="0.45">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8.2015999999999991</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="N7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="18"/>
-      <c r="P7" s="19"/>
-    </row>
-    <row r="8" spans="1:16" customFormat="1" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="9" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
+    <row r="6" spans="1:6" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="9">
+        <v>6.2015000000000002</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="1" customFormat="1" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8">
-        <v>12.202400000000001</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="171" x14ac:dyDescent="0.45">
-      <c r="A11" s="5">
-        <v>2</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="9">
-        <v>8.2014999999999993</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="5">
-        <v>3</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="9">
-        <v>8.2014999999999993</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="171" x14ac:dyDescent="0.45">
-      <c r="A13" s="5">
-        <v>4</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="9">
-        <v>8.2015999999999991</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="5">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="9">
-        <v>6.2015000000000002</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>